<commit_message>
feat: Test the sign up page
</commit_message>
<xml_diff>
--- a/src/test/resources/login_data.xlsx
+++ b/src/test/resources/login_data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SelfLearning\LearningJava\TestNGMavenExample\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2985E912-BD28-49A2-8711-A97839B7C361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E304C6-4B46-40DE-A5C0-CC56367D33CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TEMP_DATA" sheetId="3" r:id="rId1"/>
-    <sheet name="LOGIN_DATA" sheetId="1" r:id="rId2"/>
-    <sheet name="RESULT_TEST" sheetId="2" r:id="rId3"/>
+    <sheet name="LOGIN_DATA" sheetId="1" r:id="rId1"/>
+    <sheet name="SIGNUP_DATA" sheetId="4" r:id="rId2"/>
+    <sheet name="LOGIN_TEST_RESULT" sheetId="2" r:id="rId3"/>
+    <sheet name="SIGNUP_TEST_RESULT" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="56">
   <si>
     <t>Username</t>
   </si>
@@ -87,13 +88,149 @@
   </si>
   <si>
     <t>Test Time</t>
+  </si>
+  <si>
+    <t>Test login function</t>
+  </si>
+  <si>
+    <t>TestLogin</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for url to be "https://phptravels.net/dashboard". Current url: "https://phptravels.net/login" (tried for 2 second(s) with 500 milliseconds interval)
+Build info: version: '4.25.0', revision: '8a8aea2337'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.5'
+Driver info: org.openqa.selenium.edge.EdgeDriver
+Capabilities {acceptInsecureCerts: false, browserName: MicrosoftEdge, browserVersion: 130.0.2849.80, fedcm:accounts: true, ms:edgeOptions: {debuggerAddress: localhost:58839}, msedge: {msedgedriverVersion: 130.0.2849.56 (85245383cd01..., userDataDir: C:\Users\Lenovo\AppData\Loc...}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:58839/devtoo..., se:cdpVersion: 130.0.2849.80, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 47835f88f4a20d92e3b66dbe6a910a58</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for url to be "https://phptravels.net/dashboard". Current url: "https://phptravels.net/login" (tried for 2 second(s) with 500 milliseconds interval)
+Build info: version: '4.25.0', revision: '8a8aea2337'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.5'
+Driver info: org.openqa.selenium.edge.EdgeDriver
+Capabilities {acceptInsecureCerts: false, browserName: MicrosoftEdge, browserVersion: 130.0.2849.80, fedcm:accounts: true, ms:edgeOptions: {debuggerAddress: localhost:58861}, msedge: {msedgedriverVersion: 130.0.2849.56 (85245383cd01..., userDataDir: C:\Users\Lenovo\AppData\Loc...}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:58861/devtoo..., se:cdpVersion: 130.0.2849.80, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 69291f3d6e7bb46f464664386bedc175</t>
+  </si>
+  <si>
+    <t>Please include an '@' in the email address. 'a' is missing an '@'.</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for url to be "https://phptravels.net/dashboard". Current url: "https://phptravels.net/login" (tried for 2 second(s) with 500 milliseconds interval)
+Build info: version: '4.25.0', revision: '8a8aea2337'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.5'
+Driver info: org.openqa.selenium.edge.EdgeDriver
+Capabilities {acceptInsecureCerts: false, browserName: MicrosoftEdge, browserVersion: 130.0.2849.80, fedcm:accounts: true, ms:edgeOptions: {debuggerAddress: localhost:58989}, msedge: {msedgedriverVersion: 130.0.2849.56 (85245383cd01..., userDataDir: C:\Users\Lenovo\AppData\Loc...}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:58989/devtoo..., se:cdpVersion: 130.0.2849.80, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 67603a14c112c05a3ac8d5aa45d700e8</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for url to be "https://phptravels.net/dashboard". Current url: "https://phptravels.net/login" (tried for 2 second(s) with 500 milliseconds interval)
+Build info: version: '4.25.0', revision: '8a8aea2337'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.5'
+Driver info: org.openqa.selenium.edge.EdgeDriver
+Capabilities {acceptInsecureCerts: false, browserName: MicrosoftEdge, browserVersion: 130.0.2849.80, fedcm:accounts: true, ms:edgeOptions: {debuggerAddress: localhost:59014}, msedge: {msedgedriverVersion: 130.0.2849.56 (85245383cd01..., userDataDir: C:\Users\Lenovo\AppData\Loc...}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:59014/devtoo..., se:cdpVersion: 130.0.2849.80, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 5e8905e7839d137c080a7f39936bf221</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for url to be "https://phptravels.net/dashboard". Current url: "https://phptravels.net/login" (tried for 2 second(s) with 500 milliseconds interval)
+Build info: version: '4.25.0', revision: '8a8aea2337'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.5'
+Driver info: org.openqa.selenium.edge.EdgeDriver
+Capabilities {acceptInsecureCerts: false, browserName: MicrosoftEdge, browserVersion: 130.0.2849.80, fedcm:accounts: true, ms:edgeOptions: {debuggerAddress: localhost:59039}, msedge: {msedgedriverVersion: 130.0.2849.56 (85245383cd01..., userDataDir: C:\Users\Lenovo\AppData\Loc...}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:59039/devtoo..., se:cdpVersion: 130.0.2849.80, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 73e42b2f88808e9029d0284eb5a75958</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Nguyen</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>alex.nguyen240123123@gmail.com</t>
+  </si>
+  <si>
+    <t>Sign Up Success</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>john.doe@gmail.com</t>
+  </si>
+  <si>
+    <t>password123</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>michael.lee@example.com</t>
+  </si>
+  <si>
+    <t>mypassword</t>
+  </si>
+  <si>
+    <t>Sign up Success</t>
+  </si>
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
+    <t>Davis</t>
+  </si>
+  <si>
+    <t>emma.davis@gmail.com</t>
+  </si>
+  <si>
+    <t>Rachel</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>rachel.brown@example.com</t>
+  </si>
+  <si>
+    <t>securepass123</t>
+  </si>
+  <si>
+    <t>Detail Message</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="hh:mm:ss\ dd/mm/yyyy"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,16 +253,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -133,15 +282,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -422,98 +602,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DF91BCB-AAED-4CE8-9CB2-88330C613326}">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.59765625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{4A5CB3B7-BFFA-4C3A-8BD2-4CB8CD74378D}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -612,12 +705,169 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D4D8AF8-990A-4355-9A27-96D8D50FC0DD}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.8984375" customWidth="1"/>
+    <col min="2" max="2" width="13.8984375" customWidth="1"/>
+    <col min="3" max="3" width="9.59765625" customWidth="1"/>
+    <col min="4" max="4" width="9.8984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
+    <col min="6" max="6" width="21.8984375" customWidth="1"/>
+    <col min="7" max="7" width="14.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6">
+        <v>912345678</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="6">
+        <v>123456</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>987654321</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>905123440</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>876543210</v>
+      </c>
+      <c r="E6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{9CE25DB2-3E00-40DA-9056-25D51F238BA2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BBB6F8E-E071-47A0-AEF3-74C70444EECE}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:I16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -628,6 +878,7 @@
     <col min="4" max="4" width="20.5" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.8984375" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="19.69921875" customWidth="1"/>
     <col min="9" max="9" width="98.296875" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
@@ -665,6 +916,279 @@
         <v>16</v>
       </c>
     </row>
+    <row r="2" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3">
+        <v>45607.762255208334</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="3">
+        <v>45607.762351747682</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45607.762420995372</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45607.762463437502</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="3">
+        <v>45607.762569907405</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4">
+        <v>45607.762656643521</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="4">
+        <v>45607.762763923609</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{694E1B81-4059-4ED3-9874-714FF9E4BCAE}">
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:M6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="12.796875" customWidth="1"/>
+    <col min="3" max="3" width="12.19921875" customWidth="1"/>
+    <col min="4" max="4" width="11.09765625" customWidth="1"/>
+    <col min="5" max="5" width="12.8984375" customWidth="1"/>
+    <col min="6" max="6" width="15.8984375" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="12.59765625" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.09765625" customWidth="1"/>
+    <col min="12" max="12" width="13.8984375" customWidth="1"/>
+    <col min="13" max="13" width="42.19921875" customWidth="1"/>
+    <col min="14" max="14" width="98.296875" customWidth="1"/>
+    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>